<commit_message>
added contact details test case
</commit_message>
<xml_diff>
--- a/espProject/TestData/EmpData.xlsx
+++ b/espProject/TestData/EmpData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Nextgen" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="EE" sheetId="9" r:id="rId9"/>
     <sheet name="Title values" sheetId="10" r:id="rId10"/>
     <sheet name="Error Messages" sheetId="11" r:id="rId11"/>
+    <sheet name="Hire Summary Details" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="70">
   <si>
     <t>Emp First Name</t>
   </si>
@@ -231,6 +232,9 @@
   </si>
   <si>
     <t>FT/PT Indicator cannot be empty</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
   </si>
 </sst>
 </file>
@@ -812,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,6 +960,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1">
+        <v>9681317650</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>